<commit_message>
Adding index of difficulty to calc sheet
</commit_message>
<xml_diff>
--- a/Blatt03/Aufgabe05/Calculations.xlsx
+++ b/Blatt03/Aufgabe05/Calculations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Kastenbreite (px)</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Zielbreite</t>
+  </si>
+  <si>
+    <t>Index of difficulty</t>
   </si>
 </sst>
 </file>
@@ -373,15 +376,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,7 +392,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -397,7 +400,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -410,8 +413,11 @@
       <c r="D5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -427,8 +433,12 @@
         <f>$C$2 / COS(C6)</f>
         <v>63.245553203367585</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f>LOG((B6 / D6) + 1)</f>
+        <v>0.17609125905568124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -444,8 +454,12 @@
         <f t="shared" ref="D7:D9" si="2">$C$2 / COS(C7)</f>
         <v>28.284271247461898</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f t="shared" ref="E7:E9" si="3">LOG((B7 / D7) + 1)</f>
+        <v>0.3979400086720376</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -461,8 +475,12 @@
         <f t="shared" si="2"/>
         <v>23.323807579381203</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>0.54406804435027567</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -477,6 +495,10 @@
       <c r="D9">
         <f t="shared" si="2"/>
         <v>21.759351731039736</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>0.65321251377534373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>